<commit_message>
removed a view and small format changes
</commit_message>
<xml_diff>
--- a/03_export_data/patient_clinic_results.xlsx
+++ b/03_export_data/patient_clinic_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderdavis/UW/Classes/info_330su/healthcareDB/03_export_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BEDA87-9EFE-4148-91A3-9AD00511F0F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071EC8C2-6999-1744-9786-AF636FCF731D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,19 +16,16 @@
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">sheet1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">sheet1!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">sheet1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">sheet1!$B$2:$B$10</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">sheet1!$A$5:$A$13</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">sheet1!$B$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">sheet1!$B$5:$B$13</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ClinicName</t>
   </si>
@@ -62,14 +59,25 @@
   <si>
     <t>Supervalu Inc</t>
   </si>
+  <si>
+    <t>Info 330 Summer - Final Project
+Alex Davis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -84,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -92,12 +100,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,10 +230,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
+            <a:defRPr sz="1600"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -175,7 +266,26 @@
         </cx:series>
       </cx:plotAreaRegion>
     </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
+    <cx:legend pos="t" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1050"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+          </a:endParaRPr>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
   </cx:chart>
   <cx:spPr>
     <a:solidFill>
@@ -790,15 +900,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -834,8 +944,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3752850" y="165100"/>
-              <a:ext cx="6800850" cy="4546600"/>
+              <a:off x="3765550" y="825500"/>
+              <a:ext cx="6800850" cy="4381500"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -869,10 +979,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFEB78EE-2DF5-404A-8473-A46415492F2E}" name="Table1" displayName="Table1" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10" xr:uid="{3F01D42C-BF9C-D744-8105-3225A36AD7D5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
-    <sortCondition descending="1" ref="B1:B10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFEB78EE-2DF5-404A-8473-A46415492F2E}" name="Table1" displayName="Table1" ref="A4:B13" totalsRowShown="0">
+  <autoFilter ref="A4:B13" xr:uid="{3F01D42C-BF9C-D744-8105-3225A36AD7D5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:B13">
+    <sortCondition descending="1" ref="B4:B13"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1DCAC3B1-EA7D-EA44-A302-A30345B2B02A}" name="ClinicName"/>
@@ -1179,99 +1289,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
       </c>
       <c r="B5">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
+      <c r="B10">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B11">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B12">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>